<commit_message>
Deploying to gh-pages from  @ fdb56131b47a730cc7ea07becf08588c2250958a 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-4-2.xlsx
+++ b/assets/excel/2021_1-4-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFCF52E-4866-4494-B9F7-956475E74EA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906E189D-795E-4D74-B35B-0184E5664CAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{5B9D5FF7-0EDA-4F75-B44C-924FC8B4E454}"/>
   </bookViews>
@@ -31,12 +31,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
-  </si>
-  <si>
-    <t>Indikator 1.4.3: Zuzüge über die Bundesgrenzen nach Niedersachsen nach Wanderungsziel</t>
-  </si>
-  <si>
-    <t>Tabelle: 1.4.3: Zuzüge über die Bundesgrenzen nach Niedersachsen nach Wanderungsziel</t>
   </si>
   <si>
     <r>
@@ -116,6 +110,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Indikator 1.4.: Fortzüge über die Bundesgrenzen nach Niedersachsen nach Wanderungsziel</t>
+  </si>
+  <si>
+    <t>Tabelle: 1.4.2: Fortzüge über die Bundesgrenzen nach Niedersachsen nach Wanderungsziel</t>
   </si>
 </sst>
 </file>
@@ -272,27 +272,6 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -334,6 +313,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -829,7 +829,7 @@
     <row r="2" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
@@ -845,7 +845,7 @@
     </row>
     <row r="4" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -874,1735 +874,1735 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="28"/>
+    </row>
+    <row r="7" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="25"/>
+      <c r="C7" s="7">
+        <v>2005</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2006</v>
+      </c>
+      <c r="E7" s="7">
+        <v>2007</v>
+      </c>
+      <c r="F7" s="7">
+        <v>2008</v>
+      </c>
+      <c r="G7" s="7">
+        <v>2009</v>
+      </c>
+      <c r="H7" s="7">
+        <v>2010</v>
+      </c>
+      <c r="I7" s="7">
+        <v>2011</v>
+      </c>
+      <c r="J7" s="7">
+        <v>2012</v>
+      </c>
+      <c r="K7" s="7">
+        <v>2013</v>
+      </c>
+      <c r="L7" s="7">
+        <v>2014</v>
+      </c>
+      <c r="M7" s="7">
+        <v>2015</v>
+      </c>
+      <c r="N7" s="7">
+        <v>2016</v>
+      </c>
+      <c r="O7" s="7">
+        <v>2017</v>
+      </c>
+      <c r="P7" s="7">
+        <v>2018</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>2019</v>
+      </c>
+      <c r="R7" s="8">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="26"/>
+      <c r="C8" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="30"/>
+    </row>
+    <row r="9" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="9"/>
-    </row>
-    <row r="7" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="11">
-        <v>2005</v>
-      </c>
-      <c r="D7" s="11">
-        <v>2006</v>
-      </c>
-      <c r="E7" s="11">
-        <v>2007</v>
-      </c>
-      <c r="F7" s="11">
-        <v>2008</v>
-      </c>
-      <c r="G7" s="11">
-        <v>2009</v>
-      </c>
-      <c r="H7" s="11">
-        <v>2010</v>
-      </c>
-      <c r="I7" s="11">
-        <v>2011</v>
-      </c>
-      <c r="J7" s="11">
-        <v>2012</v>
-      </c>
-      <c r="K7" s="11">
-        <v>2013</v>
-      </c>
-      <c r="L7" s="11">
-        <v>2014</v>
-      </c>
-      <c r="M7" s="11">
-        <v>2015</v>
-      </c>
-      <c r="N7" s="11">
-        <v>2016</v>
-      </c>
-      <c r="O7" s="11">
-        <v>2017</v>
-      </c>
-      <c r="P7" s="11">
-        <v>2018</v>
-      </c>
-      <c r="Q7" s="11">
-        <v>2019</v>
-      </c>
-      <c r="R7" s="12">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="14" t="s">
+      <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="15"/>
-    </row>
-    <row r="9" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="D9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="E9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="F9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="G9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="H9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="I9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="J9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="K9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="L9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="M9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="N9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="O9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="P9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="17" t="s">
+      <c r="Q9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="R9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="R9" s="17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="str">
+    </row>
+    <row r="10" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B3</f>
         <v xml:space="preserve">Europa insgesamt            </v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="12">
         <v>41701</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="12">
         <v>44056</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="12">
         <v>46198</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="12">
         <v>52345</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="12">
         <v>51736</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="12">
         <v>48102</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="12">
         <v>53877</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="12">
         <v>57738</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="12">
         <v>63077</v>
       </c>
-      <c r="L10" s="19">
+      <c r="L10" s="12">
         <v>70667</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="12">
         <v>71404</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="12">
         <v>88788</v>
       </c>
-      <c r="O10" s="19">
+      <c r="O10" s="12">
         <v>74075</v>
       </c>
-      <c r="P10" s="19">
+      <c r="P10" s="12">
         <v>78856</v>
       </c>
-      <c r="Q10" s="19">
+      <c r="Q10" s="12">
         <v>81579</v>
       </c>
-      <c r="R10" s="19">
+      <c r="R10" s="12">
         <v>62401</v>
       </c>
     </row>
-    <row r="11" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B11" s="21" t="str">
+    <row r="11" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B11" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B4</f>
         <v xml:space="preserve">  Bulgarien                 </v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="15">
         <v>396</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="15">
         <v>304</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="15">
         <v>592</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="15">
         <v>1232</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="15">
         <v>1841</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="15">
         <v>2242</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="15">
         <v>2627</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="15">
         <v>2688</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="15">
         <v>2956</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="15">
         <v>3884</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="15">
         <v>3816</v>
       </c>
-      <c r="N11" s="22">
+      <c r="N11" s="15">
         <v>5272</v>
       </c>
-      <c r="O11" s="22">
+      <c r="O11" s="15">
         <v>4786</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="15">
         <v>5917</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="Q11" s="15">
         <v>6733</v>
       </c>
-      <c r="R11" s="22">
+      <c r="R11" s="15">
         <v>5255</v>
       </c>
     </row>
-    <row r="12" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B12" s="21" t="str">
+    <row r="12" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B12" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B5</f>
         <v xml:space="preserve">  Griechenland              </v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="15">
         <v>1008</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="15">
         <v>904</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="15">
         <v>832</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="15">
         <v>1049</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="15">
         <v>954</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="15">
         <v>698</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="15">
         <v>582</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="15">
         <v>732</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="15">
         <v>822</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="15">
         <v>1251</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="15">
         <v>915</v>
       </c>
-      <c r="N12" s="22">
+      <c r="N12" s="15">
         <v>1336</v>
       </c>
-      <c r="O12" s="22">
+      <c r="O12" s="15">
         <v>1197</v>
       </c>
-      <c r="P12" s="22">
+      <c r="P12" s="15">
         <v>1253</v>
       </c>
-      <c r="Q12" s="22">
+      <c r="Q12" s="15">
         <v>1378</v>
       </c>
-      <c r="R12" s="22">
+      <c r="R12" s="15">
         <v>1150</v>
       </c>
     </row>
-    <row r="13" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B13" s="21" t="str">
+    <row r="13" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B13" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B6</f>
         <v xml:space="preserve">  Italien                   </v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="15">
         <v>1375</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="15">
         <v>1280</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="15">
         <v>1226</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="15">
         <v>1359</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="15">
         <v>1320</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="15">
         <v>1232</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="15">
         <v>1460</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="15">
         <v>1227</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="15">
         <v>1448</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="15">
         <v>2196</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="15">
         <v>2040</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="15">
         <v>2521</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="15">
         <v>2241</v>
       </c>
-      <c r="P13" s="22">
+      <c r="P13" s="15">
         <v>2369</v>
       </c>
-      <c r="Q13" s="22">
+      <c r="Q13" s="15">
         <v>2546</v>
       </c>
-      <c r="R13" s="22">
+      <c r="R13" s="15">
         <v>1734</v>
       </c>
     </row>
-    <row r="14" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B14" s="21" t="str">
+    <row r="14" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B14" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B7</f>
         <v xml:space="preserve">  Kroatien                  </v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="15">
         <v>438</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="15">
         <v>352</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="15">
         <v>435</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="15">
         <v>395</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="15">
         <v>485</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="15">
         <v>312</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="15">
         <v>384</v>
       </c>
-      <c r="J14" s="22">
+      <c r="J14" s="15">
         <v>375</v>
       </c>
-      <c r="K14" s="22">
+      <c r="K14" s="15">
         <v>533</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="15">
         <v>672</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="15">
         <v>871</v>
       </c>
-      <c r="N14" s="22">
+      <c r="N14" s="15">
         <v>1119</v>
       </c>
-      <c r="O14" s="22">
+      <c r="O14" s="15">
         <v>974</v>
       </c>
-      <c r="P14" s="22">
+      <c r="P14" s="15">
         <v>1302</v>
       </c>
-      <c r="Q14" s="22">
+      <c r="Q14" s="15">
         <v>1489</v>
       </c>
-      <c r="R14" s="22">
+      <c r="R14" s="15">
         <v>1049</v>
       </c>
     </row>
-    <row r="15" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B15" s="21" t="str">
+    <row r="15" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B15" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B8</f>
         <v xml:space="preserve">  Litauen                   </v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="15">
         <v>321</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="15">
         <v>495</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="15">
         <v>571</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="15">
         <v>535</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="15">
         <v>424</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="15">
         <v>423</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="15">
         <v>688</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J15" s="15">
         <v>779</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="15">
         <v>873</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="15">
         <v>983</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="15">
         <v>735</v>
       </c>
-      <c r="N15" s="22">
+      <c r="N15" s="15">
         <v>978</v>
       </c>
-      <c r="O15" s="22">
+      <c r="O15" s="15">
         <v>907</v>
       </c>
-      <c r="P15" s="22">
+      <c r="P15" s="15">
         <v>1106</v>
       </c>
-      <c r="Q15" s="22">
+      <c r="Q15" s="15">
         <v>1408</v>
       </c>
-      <c r="R15" s="22">
+      <c r="R15" s="15">
         <v>1351</v>
       </c>
     </row>
-    <row r="16" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B16" s="21" t="str">
+    <row r="16" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B16" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B9</f>
         <v xml:space="preserve">  Moldau, Republik          </v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="15">
         <v>34</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="15">
         <v>41</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="15">
         <v>30</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="15">
         <v>31</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="15">
         <v>38</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="15">
         <v>29</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="15">
         <v>44</v>
       </c>
-      <c r="J16" s="22">
+      <c r="J16" s="15">
         <v>44</v>
       </c>
-      <c r="K16" s="22">
+      <c r="K16" s="15">
         <v>65</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="15">
         <v>98</v>
       </c>
-      <c r="M16" s="22">
+      <c r="M16" s="15">
         <v>157</v>
       </c>
-      <c r="N16" s="22">
+      <c r="N16" s="15">
         <v>369</v>
       </c>
-      <c r="O16" s="22">
+      <c r="O16" s="15">
         <v>466</v>
       </c>
-      <c r="P16" s="22">
+      <c r="P16" s="15">
         <v>844</v>
       </c>
-      <c r="Q16" s="22">
+      <c r="Q16" s="15">
         <v>1098</v>
       </c>
-      <c r="R16" s="22">
+      <c r="R16" s="15">
         <v>958</v>
       </c>
     </row>
-    <row r="17" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B17" s="21" t="str">
+    <row r="17" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B17" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B10</f>
         <v xml:space="preserve">  Niederlande               </v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="15">
         <v>1191</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="15">
         <v>1342</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="15">
         <v>1555</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="15">
         <v>1676</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="15">
         <v>1647</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="15">
         <v>1520</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="15">
         <v>1579</v>
       </c>
-      <c r="J17" s="22">
+      <c r="J17" s="15">
         <v>1576</v>
       </c>
-      <c r="K17" s="22">
+      <c r="K17" s="15">
         <v>1538</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="15">
         <v>1661</v>
       </c>
-      <c r="M17" s="22">
+      <c r="M17" s="15">
         <v>1615</v>
       </c>
-      <c r="N17" s="22">
+      <c r="N17" s="15">
         <v>1744</v>
       </c>
-      <c r="O17" s="22">
+      <c r="O17" s="15">
         <v>1657</v>
       </c>
-      <c r="P17" s="22">
+      <c r="P17" s="15">
         <v>1725</v>
       </c>
-      <c r="Q17" s="22">
+      <c r="Q17" s="15">
         <v>1891</v>
       </c>
-      <c r="R17" s="22">
+      <c r="R17" s="15">
         <v>1498</v>
       </c>
     </row>
-    <row r="18" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B18" s="21" t="str">
+    <row r="18" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B18" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B11</f>
         <v xml:space="preserve">  Österreich                </v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="15">
         <v>804</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="15">
         <v>852</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="15">
         <v>897</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="15">
         <v>1127</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="15">
         <v>1025</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="15">
         <v>859</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="15">
         <v>896</v>
       </c>
-      <c r="J18" s="22">
+      <c r="J18" s="15">
         <v>845</v>
       </c>
-      <c r="K18" s="22">
+      <c r="K18" s="15">
         <v>901</v>
       </c>
-      <c r="L18" s="22">
+      <c r="L18" s="15">
         <v>904</v>
       </c>
-      <c r="M18" s="22">
+      <c r="M18" s="15">
         <v>793</v>
       </c>
-      <c r="N18" s="22">
+      <c r="N18" s="15">
         <v>902</v>
       </c>
-      <c r="O18" s="22">
+      <c r="O18" s="15">
         <v>887</v>
       </c>
-      <c r="P18" s="22">
+      <c r="P18" s="15">
         <v>932</v>
       </c>
-      <c r="Q18" s="22">
+      <c r="Q18" s="15">
         <v>974</v>
       </c>
-      <c r="R18" s="22">
+      <c r="R18" s="15">
         <v>861</v>
       </c>
     </row>
-    <row r="19" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B19" s="21" t="str">
+    <row r="19" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B19" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B12</f>
         <v xml:space="preserve">  Polen                     </v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="15">
         <v>20880</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="15">
         <v>22721</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="15">
         <v>23694</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="15">
         <v>23944</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G19" s="15">
         <v>22459</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="15">
         <v>20217</v>
       </c>
-      <c r="I19" s="22">
+      <c r="I19" s="15">
         <v>21030</v>
       </c>
-      <c r="J19" s="22">
+      <c r="J19" s="15">
         <v>23197</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="15">
         <v>24637</v>
       </c>
-      <c r="L19" s="22">
+      <c r="L19" s="15">
         <v>24817</v>
       </c>
-      <c r="M19" s="22">
+      <c r="M19" s="15">
         <v>22535</v>
       </c>
-      <c r="N19" s="22">
+      <c r="N19" s="15">
         <v>23500</v>
       </c>
-      <c r="O19" s="22">
+      <c r="O19" s="15">
         <v>19715</v>
       </c>
-      <c r="P19" s="22">
+      <c r="P19" s="15">
         <v>19819</v>
       </c>
-      <c r="Q19" s="22">
+      <c r="Q19" s="15">
         <v>19712</v>
       </c>
-      <c r="R19" s="22">
+      <c r="R19" s="15">
         <v>14364</v>
       </c>
     </row>
-    <row r="20" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B20" s="21" t="str">
+    <row r="20" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B20" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B13</f>
         <v xml:space="preserve">  Rumänien                  </v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="15">
         <v>584</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="15">
         <v>726</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="15">
         <v>1668</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="15">
         <v>3399</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="15">
         <v>5282</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="15">
         <v>6223</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="15">
         <v>8799</v>
       </c>
-      <c r="J20" s="22">
+      <c r="J20" s="15">
         <v>10064</v>
       </c>
-      <c r="K20" s="22">
+      <c r="K20" s="15">
         <v>11001</v>
       </c>
-      <c r="L20" s="22">
+      <c r="L20" s="15">
         <v>13262</v>
       </c>
-      <c r="M20" s="22">
+      <c r="M20" s="15">
         <v>14396</v>
       </c>
-      <c r="N20" s="22">
+      <c r="N20" s="15">
         <v>19889</v>
       </c>
-      <c r="O20" s="22">
+      <c r="O20" s="15">
         <v>20284</v>
       </c>
-      <c r="P20" s="22">
+      <c r="P20" s="15">
         <v>24730</v>
       </c>
-      <c r="Q20" s="22">
+      <c r="Q20" s="15">
         <v>25445</v>
       </c>
-      <c r="R20" s="22">
+      <c r="R20" s="15">
         <v>19738</v>
       </c>
     </row>
-    <row r="21" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B21" s="21" t="str">
+    <row r="21" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B21" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B14</f>
         <v xml:space="preserve">  Schweiz                   </v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="15">
         <v>771</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="15">
         <v>1060</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="15">
         <v>1264</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="15">
         <v>1828</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="15">
         <v>1510</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="15">
         <v>1285</v>
       </c>
-      <c r="I21" s="22">
+      <c r="I21" s="15">
         <v>1391</v>
       </c>
-      <c r="J21" s="22">
+      <c r="J21" s="15">
         <v>1204</v>
       </c>
-      <c r="K21" s="22">
+      <c r="K21" s="15">
         <v>1163</v>
       </c>
-      <c r="L21" s="22">
+      <c r="L21" s="15">
         <v>1121</v>
       </c>
-      <c r="M21" s="22">
+      <c r="M21" s="15">
         <v>1078</v>
       </c>
-      <c r="N21" s="22">
+      <c r="N21" s="15">
         <v>930</v>
       </c>
-      <c r="O21" s="22">
+      <c r="O21" s="15">
         <v>906</v>
       </c>
-      <c r="P21" s="22">
+      <c r="P21" s="15">
         <v>826</v>
       </c>
-      <c r="Q21" s="22">
+      <c r="Q21" s="15">
         <v>984</v>
       </c>
-      <c r="R21" s="22">
+      <c r="R21" s="15">
         <v>770</v>
       </c>
     </row>
-    <row r="22" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B22" s="21" t="str">
+    <row r="22" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B22" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B15</f>
         <v xml:space="preserve">  Serbien     (ab 2008)</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="22">
+      <c r="C22" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="15">
         <v>193</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="15">
         <v>717</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="15">
         <v>907</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="15">
         <v>1116</v>
       </c>
-      <c r="J22" s="22">
+      <c r="J22" s="15">
         <v>1262</v>
       </c>
-      <c r="K22" s="22">
+      <c r="K22" s="15">
         <v>1248</v>
       </c>
-      <c r="L22" s="22">
+      <c r="L22" s="15">
         <v>1655</v>
       </c>
-      <c r="M22" s="22">
+      <c r="M22" s="15">
         <v>2648</v>
       </c>
-      <c r="N22" s="22">
+      <c r="N22" s="15">
         <v>3256</v>
       </c>
-      <c r="O22" s="22">
+      <c r="O22" s="15">
         <v>1385</v>
       </c>
-      <c r="P22" s="22">
+      <c r="P22" s="15">
         <v>1235</v>
       </c>
-      <c r="Q22" s="22">
+      <c r="Q22" s="15">
         <v>1152</v>
       </c>
-      <c r="R22" s="22">
+      <c r="R22" s="15">
         <v>805</v>
       </c>
     </row>
-    <row r="23" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B23" s="21" t="str">
+    <row r="23" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B23" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B16</f>
         <v xml:space="preserve">  Spanien                   </v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="15">
         <v>1446</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="15">
         <v>1649</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="15">
         <v>1504</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="15">
         <v>1707</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="15">
         <v>1486</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="15">
         <v>1320</v>
       </c>
-      <c r="I23" s="22">
+      <c r="I23" s="15">
         <v>1320</v>
       </c>
-      <c r="J23" s="22">
+      <c r="J23" s="15">
         <v>1276</v>
       </c>
-      <c r="K23" s="22">
+      <c r="K23" s="15">
         <v>1655</v>
       </c>
-      <c r="L23" s="22">
+      <c r="L23" s="15">
         <v>1957</v>
       </c>
-      <c r="M23" s="22">
+      <c r="M23" s="15">
         <v>1623</v>
       </c>
-      <c r="N23" s="22">
+      <c r="N23" s="15">
         <v>1936</v>
       </c>
-      <c r="O23" s="22">
+      <c r="O23" s="15">
         <v>1568</v>
       </c>
-      <c r="P23" s="22">
+      <c r="P23" s="15">
         <v>1715</v>
       </c>
-      <c r="Q23" s="22">
+      <c r="Q23" s="15">
         <v>1641</v>
       </c>
-      <c r="R23" s="22">
+      <c r="R23" s="15">
         <v>1173</v>
       </c>
     </row>
-    <row r="24" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B24" s="21" t="str">
+    <row r="24" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B24" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B17</f>
         <v xml:space="preserve">  Türkei                    </v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="15">
         <v>2012</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="15">
         <v>2046</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="15">
         <v>1889</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F24" s="15">
         <v>2159</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24" s="15">
         <v>2076</v>
       </c>
-      <c r="H24" s="22">
+      <c r="H24" s="15">
         <v>1817</v>
       </c>
-      <c r="I24" s="22">
+      <c r="I24" s="15">
         <v>1727</v>
       </c>
-      <c r="J24" s="22">
+      <c r="J24" s="15">
         <v>1743</v>
       </c>
-      <c r="K24" s="22">
+      <c r="K24" s="15">
         <v>1809</v>
       </c>
-      <c r="L24" s="22">
+      <c r="L24" s="15">
         <v>1821</v>
       </c>
-      <c r="M24" s="22">
+      <c r="M24" s="15">
         <v>1644</v>
       </c>
-      <c r="N24" s="22">
+      <c r="N24" s="15">
         <v>1926</v>
       </c>
-      <c r="O24" s="22">
+      <c r="O24" s="15">
         <v>1636</v>
       </c>
-      <c r="P24" s="22">
+      <c r="P24" s="15">
         <v>1901</v>
       </c>
-      <c r="Q24" s="22">
+      <c r="Q24" s="15">
         <v>1769</v>
       </c>
-      <c r="R24" s="22">
+      <c r="R24" s="15">
         <v>1395</v>
       </c>
     </row>
-    <row r="25" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B25" s="21" t="str">
+    <row r="25" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B25" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B18</f>
         <v xml:space="preserve">  Ukraine                   </v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="15">
         <v>441</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="15">
         <v>395</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="15">
         <v>329</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F25" s="15">
         <v>451</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G25" s="15">
         <v>293</v>
       </c>
-      <c r="H25" s="22">
+      <c r="H25" s="15">
         <v>242</v>
       </c>
-      <c r="I25" s="22">
+      <c r="I25" s="15">
         <v>293</v>
       </c>
-      <c r="J25" s="22">
+      <c r="J25" s="15">
         <v>261</v>
       </c>
-      <c r="K25" s="22">
+      <c r="K25" s="15">
         <v>252</v>
       </c>
-      <c r="L25" s="22">
+      <c r="L25" s="15">
         <v>284</v>
       </c>
-      <c r="M25" s="22">
+      <c r="M25" s="15">
         <v>317</v>
       </c>
-      <c r="N25" s="22">
+      <c r="N25" s="15">
         <v>478</v>
       </c>
-      <c r="O25" s="22">
+      <c r="O25" s="15">
         <v>708</v>
       </c>
-      <c r="P25" s="22">
+      <c r="P25" s="15">
         <v>683</v>
       </c>
-      <c r="Q25" s="22">
+      <c r="Q25" s="15">
         <v>1070</v>
       </c>
-      <c r="R25" s="22">
+      <c r="R25" s="15">
         <v>752</v>
       </c>
     </row>
-    <row r="26" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B26" s="21" t="str">
+    <row r="26" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B26" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B19</f>
         <v xml:space="preserve">  Ungarn                    </v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="15">
         <v>1435</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="15">
         <v>1719</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="15">
         <v>2058</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="15">
         <v>2415</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G26" s="15">
         <v>2632</v>
       </c>
-      <c r="H26" s="22">
+      <c r="H26" s="15">
         <v>2054</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I26" s="15">
         <v>2534</v>
       </c>
-      <c r="J26" s="22">
+      <c r="J26" s="15">
         <v>2651</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K26" s="15">
         <v>3419</v>
       </c>
-      <c r="L26" s="22">
+      <c r="L26" s="15">
         <v>3489</v>
       </c>
-      <c r="M26" s="22">
+      <c r="M26" s="15">
         <v>2997</v>
       </c>
-      <c r="N26" s="22">
+      <c r="N26" s="15">
         <v>3035</v>
       </c>
-      <c r="O26" s="22">
+      <c r="O26" s="15">
         <v>2765</v>
       </c>
-      <c r="P26" s="22">
+      <c r="P26" s="15">
         <v>2578</v>
       </c>
-      <c r="Q26" s="22">
+      <c r="Q26" s="15">
         <v>2332</v>
       </c>
-      <c r="R26" s="22">
+      <c r="R26" s="15">
         <v>2020</v>
       </c>
     </row>
-    <row r="27" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B27" s="21" t="str">
+    <row r="27" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B27" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B20</f>
         <v xml:space="preserve">  Vereinigtes Königreich, Nordirland</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="15">
         <v>1329</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="15">
         <v>1428</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="15">
         <v>1242</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F27" s="15">
         <v>1434</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G27" s="15">
         <v>1435</v>
       </c>
-      <c r="H27" s="22">
+      <c r="H27" s="15">
         <v>1176</v>
       </c>
-      <c r="I27" s="22">
+      <c r="I27" s="15">
         <v>1276</v>
       </c>
-      <c r="J27" s="22">
+      <c r="J27" s="15">
         <v>1177</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K27" s="15">
         <v>1227</v>
       </c>
-      <c r="L27" s="22">
+      <c r="L27" s="15">
         <v>1531</v>
       </c>
-      <c r="M27" s="22">
+      <c r="M27" s="15">
         <v>1497</v>
       </c>
-      <c r="N27" s="22">
+      <c r="N27" s="15">
         <v>1339</v>
       </c>
-      <c r="O27" s="22">
+      <c r="O27" s="15">
         <v>1090</v>
       </c>
-      <c r="P27" s="22">
+      <c r="P27" s="15">
         <v>1193</v>
       </c>
-      <c r="Q27" s="22">
+      <c r="Q27" s="15">
         <v>1200</v>
       </c>
-      <c r="R27" s="22">
+      <c r="R27" s="15">
         <v>887</v>
       </c>
     </row>
-    <row r="28" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="18" t="str">
+    <row r="28" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B21</f>
         <v xml:space="preserve"> EU Staaten                 </v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="12">
         <v>35054</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="12">
         <v>37538</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="12">
         <v>40122</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F28" s="12">
         <v>44373</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="12">
         <v>44947</v>
       </c>
-      <c r="H28" s="19">
+      <c r="H28" s="12">
         <v>41807</v>
       </c>
-      <c r="I28" s="19">
+      <c r="I28" s="12">
         <v>47208</v>
       </c>
-      <c r="J28" s="19">
+      <c r="J28" s="12">
         <v>50761</v>
       </c>
-      <c r="K28" s="19">
+      <c r="K28" s="12">
         <v>55590</v>
       </c>
-      <c r="L28" s="19">
+      <c r="L28" s="12">
         <v>61810</v>
       </c>
-      <c r="M28" s="19">
+      <c r="M28" s="12">
         <v>58568</v>
       </c>
-      <c r="N28" s="19">
+      <c r="N28" s="12">
         <v>68721</v>
       </c>
-      <c r="O28" s="19">
+      <c r="O28" s="12">
         <v>62569</v>
       </c>
-      <c r="P28" s="19">
+      <c r="P28" s="12">
         <v>69033</v>
       </c>
-      <c r="Q28" s="19">
+      <c r="Q28" s="12">
         <v>71647</v>
       </c>
-      <c r="R28" s="19">
+      <c r="R28" s="12">
         <v>55071</v>
       </c>
     </row>
-    <row r="29" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="18" t="str">
+    <row r="29" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B22</f>
         <v xml:space="preserve">Afrika insgesamt            </v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="12">
         <v>1545</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="12">
         <v>1512</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E29" s="12">
         <v>1367</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F29" s="12">
         <v>1598</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="12">
         <v>1348</v>
       </c>
-      <c r="H29" s="19">
+      <c r="H29" s="12">
         <v>1208</v>
       </c>
-      <c r="I29" s="19">
+      <c r="I29" s="12">
         <v>1259</v>
       </c>
-      <c r="J29" s="19">
+      <c r="J29" s="12">
         <v>1257</v>
       </c>
-      <c r="K29" s="19">
+      <c r="K29" s="12">
         <v>1355</v>
       </c>
-      <c r="L29" s="19">
+      <c r="L29" s="12">
         <v>2023</v>
       </c>
-      <c r="M29" s="19">
+      <c r="M29" s="12">
         <v>2438</v>
       </c>
-      <c r="N29" s="19">
+      <c r="N29" s="12">
         <v>6689</v>
       </c>
-      <c r="O29" s="19">
+      <c r="O29" s="12">
         <v>4200</v>
       </c>
-      <c r="P29" s="19">
+      <c r="P29" s="12">
         <v>2701</v>
       </c>
-      <c r="Q29" s="19">
+      <c r="Q29" s="12">
         <v>2560</v>
       </c>
-      <c r="R29" s="19">
+      <c r="R29" s="12">
         <v>2013</v>
       </c>
     </row>
-    <row r="30" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B30" s="18" t="str">
+    <row r="30" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B23</f>
         <v xml:space="preserve">Amerika insgesamt           </v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="12">
         <v>3678</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="12">
         <v>3627</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="12">
         <v>4031</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F30" s="12">
         <v>5228</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="12">
         <v>4375</v>
       </c>
-      <c r="H30" s="19">
+      <c r="H30" s="12">
         <v>4047</v>
       </c>
-      <c r="I30" s="19">
+      <c r="I30" s="12">
         <v>4034</v>
       </c>
-      <c r="J30" s="19">
+      <c r="J30" s="12">
         <v>3832</v>
       </c>
-      <c r="K30" s="19">
+      <c r="K30" s="12">
         <v>3847</v>
       </c>
-      <c r="L30" s="19">
+      <c r="L30" s="12">
         <v>4067</v>
       </c>
-      <c r="M30" s="19">
+      <c r="M30" s="12">
         <v>3859</v>
       </c>
-      <c r="N30" s="19">
+      <c r="N30" s="12">
         <v>4286</v>
       </c>
-      <c r="O30" s="19">
+      <c r="O30" s="12">
         <v>3611</v>
       </c>
-      <c r="P30" s="19">
+      <c r="P30" s="12">
         <v>3577</v>
       </c>
-      <c r="Q30" s="19">
+      <c r="Q30" s="12">
         <v>3820</v>
       </c>
-      <c r="R30" s="19">
+      <c r="R30" s="12">
         <v>2624</v>
       </c>
     </row>
-    <row r="31" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B31" s="21" t="str">
+    <row r="31" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B31" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B24</f>
         <v xml:space="preserve">  Vereinigte Staaten        </v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="15">
         <v>1677</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="15">
         <v>1584</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E31" s="15">
         <v>1604</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="15">
         <v>1972</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G31" s="15">
         <v>1844</v>
       </c>
-      <c r="H31" s="22">
+      <c r="H31" s="15">
         <v>1698</v>
       </c>
-      <c r="I31" s="22">
+      <c r="I31" s="15">
         <v>1785</v>
       </c>
-      <c r="J31" s="22">
+      <c r="J31" s="15">
         <v>1767</v>
       </c>
-      <c r="K31" s="22">
+      <c r="K31" s="15">
         <v>1641</v>
       </c>
-      <c r="L31" s="22">
+      <c r="L31" s="15">
         <v>1828</v>
       </c>
-      <c r="M31" s="22">
+      <c r="M31" s="15">
         <v>1637</v>
       </c>
-      <c r="N31" s="22">
+      <c r="N31" s="15">
         <v>1847</v>
       </c>
-      <c r="O31" s="22">
+      <c r="O31" s="15">
         <v>1556</v>
       </c>
-      <c r="P31" s="22">
+      <c r="P31" s="15">
         <v>1446</v>
       </c>
-      <c r="Q31" s="22">
+      <c r="Q31" s="15">
         <v>1482</v>
       </c>
-      <c r="R31" s="22">
+      <c r="R31" s="15">
         <v>958</v>
       </c>
     </row>
-    <row r="32" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B32" s="18" t="str">
+    <row r="32" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B25</f>
         <v xml:space="preserve">Asien insgesamt             </v>
       </c>
-      <c r="C32" s="19">
+      <c r="C32" s="12">
         <v>5059</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D32" s="12">
         <v>4600</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="12">
         <v>4615</v>
       </c>
-      <c r="F32" s="19">
+      <c r="F32" s="12">
         <v>5596</v>
       </c>
-      <c r="G32" s="19">
+      <c r="G32" s="12">
         <v>5258</v>
       </c>
-      <c r="H32" s="19">
+      <c r="H32" s="12">
         <v>5517</v>
       </c>
-      <c r="I32" s="19">
+      <c r="I32" s="12">
         <v>5517</v>
       </c>
-      <c r="J32" s="19">
+      <c r="J32" s="12">
         <v>5342</v>
       </c>
-      <c r="K32" s="19">
+      <c r="K32" s="12">
         <v>5163</v>
       </c>
-      <c r="L32" s="19">
+      <c r="L32" s="12">
         <v>5882</v>
       </c>
-      <c r="M32" s="19">
+      <c r="M32" s="12">
         <v>5817</v>
       </c>
-      <c r="N32" s="19">
+      <c r="N32" s="12">
         <v>7351</v>
       </c>
-      <c r="O32" s="19">
+      <c r="O32" s="12">
         <v>5946</v>
       </c>
-      <c r="P32" s="19">
+      <c r="P32" s="12">
         <v>6360</v>
       </c>
-      <c r="Q32" s="19">
+      <c r="Q32" s="12">
         <v>6229</v>
       </c>
-      <c r="R32" s="19">
+      <c r="R32" s="12">
         <v>4526</v>
       </c>
     </row>
-    <row r="33" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B33" s="21" t="str">
+    <row r="33" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B33" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B26</f>
         <v xml:space="preserve">  China                     </v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33" s="15">
         <v>962</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="15">
         <v>937</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33" s="15">
         <v>858</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="15">
         <v>1235</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G33" s="15">
         <v>1033</v>
       </c>
-      <c r="H33" s="22">
+      <c r="H33" s="15">
         <v>1166</v>
       </c>
-      <c r="I33" s="22">
+      <c r="I33" s="15">
         <v>1113</v>
       </c>
-      <c r="J33" s="22">
+      <c r="J33" s="15">
         <v>1087</v>
       </c>
-      <c r="K33" s="22">
+      <c r="K33" s="15">
         <v>1087</v>
       </c>
-      <c r="L33" s="22">
+      <c r="L33" s="15">
         <v>1287</v>
       </c>
-      <c r="M33" s="22">
+      <c r="M33" s="15">
         <v>1371</v>
       </c>
-      <c r="N33" s="22">
+      <c r="N33" s="15">
         <v>1499</v>
       </c>
-      <c r="O33" s="22">
+      <c r="O33" s="15">
         <v>1469</v>
       </c>
-      <c r="P33" s="22">
+      <c r="P33" s="15">
         <v>1522</v>
       </c>
-      <c r="Q33" s="22">
+      <c r="Q33" s="15">
         <v>1559</v>
       </c>
-      <c r="R33" s="22">
+      <c r="R33" s="15">
         <v>1309</v>
       </c>
     </row>
-    <row r="34" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B34" s="18" t="str">
+    <row r="34" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B27</f>
         <v xml:space="preserve">Australien und Ozeanien     </v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="12">
         <v>396</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D34" s="12">
         <v>413</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E34" s="12">
         <v>502</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F34" s="12">
         <v>608</v>
       </c>
-      <c r="G34" s="19">
+      <c r="G34" s="12">
         <v>562</v>
       </c>
-      <c r="H34" s="19">
+      <c r="H34" s="12">
         <v>547</v>
       </c>
-      <c r="I34" s="19">
+      <c r="I34" s="12">
         <v>535</v>
       </c>
-      <c r="J34" s="19">
+      <c r="J34" s="12">
         <v>500</v>
       </c>
-      <c r="K34" s="19">
+      <c r="K34" s="12">
         <v>554</v>
       </c>
-      <c r="L34" s="19">
+      <c r="L34" s="12">
         <v>572</v>
       </c>
-      <c r="M34" s="19">
+      <c r="M34" s="12">
         <v>531</v>
       </c>
-      <c r="N34" s="19">
+      <c r="N34" s="12">
         <v>593</v>
       </c>
-      <c r="O34" s="19">
+      <c r="O34" s="12">
         <v>566</v>
       </c>
-      <c r="P34" s="19">
+      <c r="P34" s="12">
         <v>524</v>
       </c>
-      <c r="Q34" s="19">
+      <c r="Q34" s="12">
         <v>497</v>
       </c>
-      <c r="R34" s="19">
+      <c r="R34" s="12">
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B35" s="21" t="str">
+    <row r="35" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B35" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B28</f>
         <v xml:space="preserve">Sonstige Ziele              </v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="15">
         <v>2997</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="15">
         <v>2129</v>
       </c>
-      <c r="E35" s="22">
+      <c r="E35" s="15">
         <v>2314</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="15">
         <v>2739</v>
       </c>
-      <c r="G35" s="22">
+      <c r="G35" s="15">
         <v>3003</v>
       </c>
-      <c r="H35" s="22">
+      <c r="H35" s="15">
         <v>2904</v>
       </c>
-      <c r="I35" s="22">
+      <c r="I35" s="15">
         <v>2615</v>
       </c>
-      <c r="J35" s="22">
+      <c r="J35" s="15">
         <v>2812</v>
       </c>
-      <c r="K35" s="22">
+      <c r="K35" s="15">
         <v>1990</v>
       </c>
-      <c r="L35" s="22">
+      <c r="L35" s="15">
         <v>1927</v>
       </c>
-      <c r="M35" s="22">
+      <c r="M35" s="15">
         <v>3002</v>
       </c>
-      <c r="N35" s="22">
+      <c r="N35" s="15">
         <v>29314</v>
       </c>
-      <c r="O35" s="22">
+      <c r="O35" s="15">
         <v>18898</v>
       </c>
-      <c r="P35" s="22">
+      <c r="P35" s="15">
         <v>17345</v>
       </c>
-      <c r="Q35" s="22">
+      <c r="Q35" s="15">
         <v>18248</v>
       </c>
-      <c r="R35" s="22">
+      <c r="R35" s="15">
         <v>14276</v>
       </c>
     </row>
-    <row r="36" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B36" s="21" t="str">
+    <row r="36" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B36" s="14" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B29</f>
         <v xml:space="preserve">  ohne Angabe               </v>
       </c>
-      <c r="C36" s="22">
+      <c r="C36" s="15">
         <v>0</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="15">
         <v>7</v>
       </c>
-      <c r="E36" s="22">
+      <c r="E36" s="15">
         <v>2</v>
       </c>
-      <c r="F36" s="22">
+      <c r="F36" s="15">
         <v>8</v>
       </c>
-      <c r="G36" s="22">
+      <c r="G36" s="15">
         <v>19</v>
       </c>
-      <c r="H36" s="22">
+      <c r="H36" s="15">
         <v>9</v>
       </c>
-      <c r="I36" s="22">
+      <c r="I36" s="15">
         <v>43</v>
       </c>
-      <c r="J36" s="22">
+      <c r="J36" s="15">
         <v>57</v>
       </c>
-      <c r="K36" s="22">
+      <c r="K36" s="15">
         <v>61</v>
       </c>
-      <c r="L36" s="22">
+      <c r="L36" s="15">
         <v>20</v>
       </c>
-      <c r="M36" s="22">
+      <c r="M36" s="15">
         <v>1548</v>
       </c>
-      <c r="N36" s="22">
+      <c r="N36" s="15">
         <v>26271</v>
       </c>
-      <c r="O36" s="22">
+      <c r="O36" s="15">
         <v>17357</v>
       </c>
-      <c r="P36" s="22">
+      <c r="P36" s="15">
         <v>16512</v>
       </c>
-      <c r="Q36" s="22">
+      <c r="Q36" s="15">
         <v>17373</v>
       </c>
-      <c r="R36" s="22">
+      <c r="R36" s="15">
         <v>13852</v>
       </c>
     </row>
-    <row r="37" spans="2:18" s="20" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="18" t="str">
+    <row r="37" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B37" s="11" t="str">
         <f>'[1]2020_1-4-3_Rohdaten'!B30</f>
         <v xml:space="preserve">Insgesamt                   </v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="12">
         <v>55376</v>
       </c>
-      <c r="D37" s="19">
+      <c r="D37" s="12">
         <v>56337</v>
       </c>
-      <c r="E37" s="19">
+      <c r="E37" s="12">
         <v>59027</v>
       </c>
-      <c r="F37" s="19">
+      <c r="F37" s="12">
         <v>68114</v>
       </c>
-      <c r="G37" s="19">
+      <c r="G37" s="12">
         <v>66282</v>
       </c>
-      <c r="H37" s="19">
+      <c r="H37" s="12">
         <v>62325</v>
       </c>
-      <c r="I37" s="19">
+      <c r="I37" s="12">
         <v>67837</v>
       </c>
-      <c r="J37" s="19">
+      <c r="J37" s="12">
         <v>71481</v>
       </c>
-      <c r="K37" s="19">
+      <c r="K37" s="12">
         <v>75986</v>
       </c>
-      <c r="L37" s="19">
+      <c r="L37" s="12">
         <v>85138</v>
       </c>
-      <c r="M37" s="19">
+      <c r="M37" s="12">
         <v>87051</v>
       </c>
-      <c r="N37" s="19">
+      <c r="N37" s="12">
         <v>137021</v>
       </c>
-      <c r="O37" s="19">
+      <c r="O37" s="12">
         <v>107296</v>
       </c>
-      <c r="P37" s="19">
+      <c r="P37" s="12">
         <v>109363</v>
       </c>
-      <c r="Q37" s="19">
+      <c r="Q37" s="12">
         <v>112933</v>
       </c>
-      <c r="R37" s="19">
+      <c r="R37" s="12">
         <v>86127</v>
       </c>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B38" s="24"/>
-    </row>
-    <row r="39" spans="2:18" s="25" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="26"/>
-      <c r="M39" s="26"/>
-      <c r="N39" s="26"/>
-      <c r="Q39" s="27"/>
-    </row>
-    <row r="40" spans="2:18" s="25" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D40" s="26"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="28"/>
-      <c r="O40" s="28"/>
-      <c r="P40" s="28"/>
-      <c r="Q40" s="27"/>
-    </row>
-    <row r="41" spans="2:18" s="25" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="28"/>
-      <c r="N41" s="28"/>
-      <c r="O41" s="28"/>
-      <c r="P41" s="28"/>
-      <c r="Q41" s="27"/>
-    </row>
-    <row r="42" spans="2:18" s="25" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="28"/>
-      <c r="O42" s="28"/>
-      <c r="P42" s="28"/>
-      <c r="Q42" s="27"/>
+      <c r="B38" s="17"/>
+    </row>
+    <row r="39" spans="2:18" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="Q39" s="20"/>
+    </row>
+    <row r="40" spans="2:18" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="19"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="20"/>
+    </row>
+    <row r="41" spans="2:18" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="23"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="20"/>
+    </row>
+    <row r="42" spans="2:18" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 28e4540854550229be53f49aa195f655ad8818a7 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-4-2.xlsx
+++ b/assets/excel/2021_1-4-2.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906E189D-795E-4D74-B35B-0184E5664CAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D1029D-7521-4FF3-B7FE-BB295010CB0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{5B9D5FF7-0EDA-4F75-B44C-924FC8B4E454}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,13 +25,166 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
   <si>
+    <t>Fortzüge über die Bundesgrenzen aus Niedersachsen</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Quelle: Wanderungsstatistik</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Indikator 1.4.: Fortzüge über die Bundesgrenzen nach Niedersachsen nach Wanderungsziel</t>
+  </si>
+  <si>
+    <t>Tabelle: 1.4.2: Fortzüge über die Bundesgrenzen nach Niedersachsen nach Wanderungsziel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Europa insgesamt            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Albanien                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Bulgarien                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Griechenland              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Italien                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kosovo                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Moldau, Republik          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Polen                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Rumänien                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Russische Föderation      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Serbien  (ab 2008)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Spanien                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Türkei                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ukraine                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EU Staaten                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afrika insgesamt            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amerika insgesamt           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asien insgesamt             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Afghanistan               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Indien                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Irak                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Iran,Islamische Republik  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kasachstan                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Libanon                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Syrien, Arabische Republik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australien und Ozeanien     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonstige Ziele              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insgesamt                   </t>
+  </si>
+  <si>
     <r>
-      <t>Wanderungsherkunft</t>
+      <t>Wanderungsziel</t>
     </r>
     <r>
       <rPr>
@@ -46,76 +196,7 @@
     </r>
   </si>
   <si>
-    <t>Fortzüge über die Bundesgrenzen aus Niedersachsen</t>
-  </si>
-  <si>
-    <t>Anzahl</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>1) Aufgeführt sind die 20 häufigsten Wanderungsziele im Jahr 2019 als darunter Positionen der in der Zeile Ingesamt augewiesenen Werte "Staatenlos" sowie "ungeklärt und ohne Angabe" werden in Sonstige Ziele geführt.</t>
-  </si>
-  <si>
-    <t>Quelle: Wanderungsstatistik</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Indikator 1.4.: Fortzüge über die Bundesgrenzen nach Niedersachsen nach Wanderungsziel</t>
-  </si>
-  <si>
-    <t>Tabelle: 1.4.2: Fortzüge über die Bundesgrenzen nach Niedersachsen nach Wanderungsziel</t>
+    <t>1) Aufgeführt sind die 20 häufigsten Wanderungsziele im Jahr 2020 als darunter Positionen der in der Zeile Ingesamt augewiesenen Werte "Staatenlos" sowie "ungeklärt und ohne Angabe" werden in Sonstige Ziele geführt.</t>
   </si>
 </sst>
 </file>
@@ -254,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -334,6 +415,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -349,166 +444,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="2020_1-4-3_Download"/>
-      <sheetName val="2020_1-4-3_Rohdaten"/>
-      <sheetName val="2020_1-4-3_CSV_Vorbereitung"/>
-      <sheetName val="2020_1-4-3_CSV_Export"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="3">
-          <cell r="B3" t="str">
-            <v xml:space="preserve">Europa insgesamt            </v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v xml:space="preserve">  Bulgarien                 </v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v xml:space="preserve">  Griechenland              </v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v xml:space="preserve">  Italien                   </v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v xml:space="preserve">  Kroatien                  </v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8" t="str">
-            <v xml:space="preserve">  Litauen                   </v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="str">
-            <v xml:space="preserve">  Moldau, Republik          </v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v xml:space="preserve">  Niederlande               </v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v xml:space="preserve">  Österreich                </v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12" t="str">
-            <v xml:space="preserve">  Polen                     </v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v xml:space="preserve">  Rumänien                  </v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14" t="str">
-            <v xml:space="preserve">  Schweiz                   </v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15" t="str">
-            <v xml:space="preserve">  Serbien     (ab 2008)</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16" t="str">
-            <v xml:space="preserve">  Spanien                   </v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v xml:space="preserve">  Türkei                    </v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18" t="str">
-            <v xml:space="preserve">  Ukraine                   </v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19" t="str">
-            <v xml:space="preserve">  Ungarn                    </v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20" t="str">
-            <v xml:space="preserve">  Vereinigtes Königreich, Nordirland</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21" t="str">
-            <v xml:space="preserve"> EU Staaten                 </v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22" t="str">
-            <v xml:space="preserve">Afrika insgesamt            </v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23" t="str">
-            <v xml:space="preserve">Amerika insgesamt           </v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24" t="str">
-            <v xml:space="preserve">  Vereinigte Staaten        </v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25" t="str">
-            <v xml:space="preserve">Asien insgesamt             </v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26" t="str">
-            <v xml:space="preserve">  China                     </v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27" t="str">
-            <v xml:space="preserve">Australien und Ozeanien     </v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28" t="str">
-            <v xml:space="preserve">Sonstige Ziele              </v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29" t="str">
-            <v xml:space="preserve">  ohne Angabe               </v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30" t="str">
-            <v xml:space="preserve">Insgesamt                   </v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -812,7 +747,7 @@
   <dimension ref="B1:R42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +764,7 @@
     <row r="2" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
@@ -845,7 +780,7 @@
     </row>
     <row r="4" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -875,10 +810,10 @@
     </row>
     <row r="6" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>1</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>2</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
@@ -950,7 +885,7 @@
     <row r="8" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="26"/>
       <c r="C8" s="29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
@@ -970,61 +905,60 @@
     </row>
     <row r="9" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="K9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="L9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="M9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="N9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="O9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O9" s="10" t="s">
+      <c r="P9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="9" t="s">
+      <c r="Q9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="10" t="s">
+      <c r="R9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="R9" s="10" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="10" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B3</f>
-        <v xml:space="preserve">Europa insgesamt            </v>
+      <c r="B10" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="C10" s="12">
         <v>41701</v>
@@ -1076,9 +1010,8 @@
       </c>
     </row>
     <row r="11" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B11" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B4</f>
-        <v xml:space="preserve">  Bulgarien                 </v>
+      <c r="B11" s="14" t="s">
+        <v>25</v>
       </c>
       <c r="C11" s="15">
         <v>396</v>
@@ -1130,9 +1063,8 @@
       </c>
     </row>
     <row r="12" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B12" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B5</f>
-        <v xml:space="preserve">  Griechenland              </v>
+      <c r="B12" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="C12" s="15">
         <v>1008</v>
@@ -1184,9 +1116,8 @@
       </c>
     </row>
     <row r="13" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B13" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B6</f>
-        <v xml:space="preserve">  Italien                   </v>
+      <c r="B13" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="C13" s="15">
         <v>1375</v>
@@ -1238,9 +1169,8 @@
       </c>
     </row>
     <row r="14" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B14" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B7</f>
-        <v xml:space="preserve">  Kroatien                  </v>
+      <c r="B14" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="C14" s="15">
         <v>438</v>
@@ -1292,9 +1222,8 @@
       </c>
     </row>
     <row r="15" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B15" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B8</f>
-        <v xml:space="preserve">  Litauen                   </v>
+      <c r="B15" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="C15" s="15">
         <v>321</v>
@@ -1346,9 +1275,8 @@
       </c>
     </row>
     <row r="16" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B16" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B9</f>
-        <v xml:space="preserve">  Moldau, Republik          </v>
+      <c r="B16" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="C16" s="15">
         <v>34</v>
@@ -1400,9 +1328,8 @@
       </c>
     </row>
     <row r="17" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B17" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B10</f>
-        <v xml:space="preserve">  Niederlande               </v>
+      <c r="B17" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="C17" s="15">
         <v>1191</v>
@@ -1454,9 +1381,8 @@
       </c>
     </row>
     <row r="18" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B18" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B11</f>
-        <v xml:space="preserve">  Österreich                </v>
+      <c r="B18" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="C18" s="15">
         <v>804</v>
@@ -1508,9 +1434,8 @@
       </c>
     </row>
     <row r="19" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B19" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B12</f>
-        <v xml:space="preserve">  Polen                     </v>
+      <c r="B19" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="C19" s="15">
         <v>20880</v>
@@ -1562,9 +1487,8 @@
       </c>
     </row>
     <row r="20" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B20" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B13</f>
-        <v xml:space="preserve">  Rumänien                  </v>
+      <c r="B20" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="C20" s="15">
         <v>584</v>
@@ -1616,9 +1540,8 @@
       </c>
     </row>
     <row r="21" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B21" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B14</f>
-        <v xml:space="preserve">  Schweiz                   </v>
+      <c r="B21" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="C21" s="15">
         <v>771</v>
@@ -1670,18 +1593,17 @@
       </c>
     </row>
     <row r="22" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B22" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B15</f>
-        <v xml:space="preserve">  Serbien     (ab 2008)</v>
+      <c r="B22" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F22" s="15">
         <v>193</v>
@@ -1724,9 +1646,8 @@
       </c>
     </row>
     <row r="23" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B23" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B16</f>
-        <v xml:space="preserve">  Spanien                   </v>
+      <c r="B23" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="C23" s="15">
         <v>1446</v>
@@ -1777,388 +1698,380 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="24" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B24" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B17</f>
-        <v xml:space="preserve">  Türkei                    </v>
-      </c>
-      <c r="C24" s="15">
+    <row r="24" spans="2:18" s="36" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B24" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="35">
         <v>2012</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="35">
         <v>2046</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="35">
         <v>1889</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="35">
         <v>2159</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="35">
         <v>2076</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="35">
         <v>1817</v>
       </c>
-      <c r="I24" s="15">
+      <c r="I24" s="35">
         <v>1727</v>
       </c>
-      <c r="J24" s="15">
+      <c r="J24" s="35">
         <v>1743</v>
       </c>
-      <c r="K24" s="15">
+      <c r="K24" s="35">
         <v>1809</v>
       </c>
-      <c r="L24" s="15">
+      <c r="L24" s="35">
         <v>1821</v>
       </c>
-      <c r="M24" s="15">
+      <c r="M24" s="35">
         <v>1644</v>
       </c>
-      <c r="N24" s="15">
+      <c r="N24" s="35">
         <v>1926</v>
       </c>
-      <c r="O24" s="15">
+      <c r="O24" s="35">
         <v>1636</v>
       </c>
-      <c r="P24" s="15">
+      <c r="P24" s="35">
         <v>1901</v>
       </c>
-      <c r="Q24" s="15">
+      <c r="Q24" s="35">
         <v>1769</v>
       </c>
-      <c r="R24" s="15">
+      <c r="R24" s="35">
         <v>1395</v>
       </c>
     </row>
-    <row r="25" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B25" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B18</f>
-        <v xml:space="preserve">  Ukraine                   </v>
-      </c>
-      <c r="C25" s="15">
+    <row r="25" spans="2:18" s="36" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B25" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="35">
         <v>441</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="35">
         <v>395</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="35">
         <v>329</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="35">
         <v>451</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="35">
         <v>293</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="35">
         <v>242</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="35">
         <v>293</v>
       </c>
-      <c r="J25" s="15">
+      <c r="J25" s="35">
         <v>261</v>
       </c>
-      <c r="K25" s="15">
+      <c r="K25" s="35">
         <v>252</v>
       </c>
-      <c r="L25" s="15">
+      <c r="L25" s="35">
         <v>284</v>
       </c>
-      <c r="M25" s="15">
+      <c r="M25" s="35">
         <v>317</v>
       </c>
-      <c r="N25" s="15">
+      <c r="N25" s="35">
         <v>478</v>
       </c>
-      <c r="O25" s="15">
+      <c r="O25" s="35">
         <v>708</v>
       </c>
-      <c r="P25" s="15">
+      <c r="P25" s="35">
         <v>683</v>
       </c>
-      <c r="Q25" s="15">
+      <c r="Q25" s="35">
         <v>1070</v>
       </c>
-      <c r="R25" s="15">
+      <c r="R25" s="35">
         <v>752</v>
       </c>
     </row>
-    <row r="26" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B26" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B19</f>
-        <v xml:space="preserve">  Ungarn                    </v>
-      </c>
-      <c r="C26" s="15">
+    <row r="26" spans="2:18" s="36" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B26" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="35">
         <v>1435</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="35">
         <v>1719</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="35">
         <v>2058</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="35">
         <v>2415</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="35">
         <v>2632</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H26" s="35">
         <v>2054</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="35">
         <v>2534</v>
       </c>
-      <c r="J26" s="15">
+      <c r="J26" s="35">
         <v>2651</v>
       </c>
-      <c r="K26" s="15">
+      <c r="K26" s="35">
         <v>3419</v>
       </c>
-      <c r="L26" s="15">
+      <c r="L26" s="35">
         <v>3489</v>
       </c>
-      <c r="M26" s="15">
+      <c r="M26" s="35">
         <v>2997</v>
       </c>
-      <c r="N26" s="15">
+      <c r="N26" s="35">
         <v>3035</v>
       </c>
-      <c r="O26" s="15">
+      <c r="O26" s="35">
         <v>2765</v>
       </c>
-      <c r="P26" s="15">
+      <c r="P26" s="35">
         <v>2578</v>
       </c>
-      <c r="Q26" s="15">
+      <c r="Q26" s="35">
         <v>2332</v>
       </c>
-      <c r="R26" s="15">
+      <c r="R26" s="35">
         <v>2020</v>
       </c>
     </row>
-    <row r="27" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B27" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B20</f>
-        <v xml:space="preserve">  Vereinigtes Königreich, Nordirland</v>
-      </c>
-      <c r="C27" s="15">
+    <row r="27" spans="2:18" s="36" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B27" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="35">
         <v>1329</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="35">
         <v>1428</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="35">
         <v>1242</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="35">
         <v>1434</v>
       </c>
-      <c r="G27" s="15">
+      <c r="G27" s="35">
         <v>1435</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="35">
         <v>1176</v>
       </c>
-      <c r="I27" s="15">
+      <c r="I27" s="35">
         <v>1276</v>
       </c>
-      <c r="J27" s="15">
+      <c r="J27" s="35">
         <v>1177</v>
       </c>
-      <c r="K27" s="15">
+      <c r="K27" s="35">
         <v>1227</v>
       </c>
-      <c r="L27" s="15">
+      <c r="L27" s="35">
         <v>1531</v>
       </c>
-      <c r="M27" s="15">
+      <c r="M27" s="35">
         <v>1497</v>
       </c>
-      <c r="N27" s="15">
+      <c r="N27" s="35">
         <v>1339</v>
       </c>
-      <c r="O27" s="15">
+      <c r="O27" s="35">
         <v>1090</v>
       </c>
-      <c r="P27" s="15">
+      <c r="P27" s="35">
         <v>1193</v>
       </c>
-      <c r="Q27" s="15">
+      <c r="Q27" s="35">
         <v>1200</v>
       </c>
-      <c r="R27" s="15">
+      <c r="R27" s="35">
         <v>887</v>
       </c>
     </row>
-    <row r="28" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B21</f>
-        <v xml:space="preserve"> EU Staaten                 </v>
-      </c>
-      <c r="C28" s="12">
+    <row r="28" spans="2:18" s="33" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="32">
         <v>35054</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="32">
         <v>37538</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="32">
         <v>40122</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="32">
         <v>44373</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="32">
         <v>44947</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="32">
         <v>41807</v>
       </c>
-      <c r="I28" s="12">
+      <c r="I28" s="32">
         <v>47208</v>
       </c>
-      <c r="J28" s="12">
+      <c r="J28" s="32">
         <v>50761</v>
       </c>
-      <c r="K28" s="12">
+      <c r="K28" s="32">
         <v>55590</v>
       </c>
-      <c r="L28" s="12">
+      <c r="L28" s="32">
         <v>61810</v>
       </c>
-      <c r="M28" s="12">
+      <c r="M28" s="32">
         <v>58568</v>
       </c>
-      <c r="N28" s="12">
+      <c r="N28" s="32">
         <v>68721</v>
       </c>
-      <c r="O28" s="12">
+      <c r="O28" s="32">
         <v>62569</v>
       </c>
-      <c r="P28" s="12">
+      <c r="P28" s="32">
         <v>69033</v>
       </c>
-      <c r="Q28" s="12">
+      <c r="Q28" s="32">
         <v>71647</v>
       </c>
-      <c r="R28" s="12">
+      <c r="R28" s="32">
         <v>55071</v>
       </c>
     </row>
-    <row r="29" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B22</f>
-        <v xml:space="preserve">Afrika insgesamt            </v>
-      </c>
-      <c r="C29" s="12">
+    <row r="29" spans="2:18" s="33" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="32">
         <v>1545</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="32">
         <v>1512</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="32">
         <v>1367</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="32">
         <v>1598</v>
       </c>
-      <c r="G29" s="12">
+      <c r="G29" s="32">
         <v>1348</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H29" s="32">
         <v>1208</v>
       </c>
-      <c r="I29" s="12">
+      <c r="I29" s="32">
         <v>1259</v>
       </c>
-      <c r="J29" s="12">
+      <c r="J29" s="32">
         <v>1257</v>
       </c>
-      <c r="K29" s="12">
+      <c r="K29" s="32">
         <v>1355</v>
       </c>
-      <c r="L29" s="12">
+      <c r="L29" s="32">
         <v>2023</v>
       </c>
-      <c r="M29" s="12">
+      <c r="M29" s="32">
         <v>2438</v>
       </c>
-      <c r="N29" s="12">
+      <c r="N29" s="32">
         <v>6689</v>
       </c>
-      <c r="O29" s="12">
+      <c r="O29" s="32">
         <v>4200</v>
       </c>
-      <c r="P29" s="12">
+      <c r="P29" s="32">
         <v>2701</v>
       </c>
-      <c r="Q29" s="12">
+      <c r="Q29" s="32">
         <v>2560</v>
       </c>
-      <c r="R29" s="12">
+      <c r="R29" s="32">
         <v>2013</v>
       </c>
     </row>
-    <row r="30" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B23</f>
-        <v xml:space="preserve">Amerika insgesamt           </v>
-      </c>
-      <c r="C30" s="12">
+    <row r="30" spans="2:18" s="33" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="32">
         <v>3678</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="32">
         <v>3627</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="32">
         <v>4031</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="32">
         <v>5228</v>
       </c>
-      <c r="G30" s="12">
+      <c r="G30" s="32">
         <v>4375</v>
       </c>
-      <c r="H30" s="12">
+      <c r="H30" s="32">
         <v>4047</v>
       </c>
-      <c r="I30" s="12">
+      <c r="I30" s="32">
         <v>4034</v>
       </c>
-      <c r="J30" s="12">
+      <c r="J30" s="32">
         <v>3832</v>
       </c>
-      <c r="K30" s="12">
+      <c r="K30" s="32">
         <v>3847</v>
       </c>
-      <c r="L30" s="12">
+      <c r="L30" s="32">
         <v>4067</v>
       </c>
-      <c r="M30" s="12">
+      <c r="M30" s="32">
         <v>3859</v>
       </c>
-      <c r="N30" s="12">
+      <c r="N30" s="32">
         <v>4286</v>
       </c>
-      <c r="O30" s="12">
+      <c r="O30" s="32">
         <v>3611</v>
       </c>
-      <c r="P30" s="12">
+      <c r="P30" s="32">
         <v>3577</v>
       </c>
-      <c r="Q30" s="12">
+      <c r="Q30" s="32">
         <v>3820</v>
       </c>
-      <c r="R30" s="12">
+      <c r="R30" s="32">
         <v>2624</v>
       </c>
     </row>
     <row r="31" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B31" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B24</f>
-        <v xml:space="preserve">  Vereinigte Staaten        </v>
+      <c r="B31" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="C31" s="15">
         <v>1677</v>
@@ -2209,64 +2122,62 @@
         <v>958</v>
       </c>
     </row>
-    <row r="32" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B25</f>
-        <v xml:space="preserve">Asien insgesamt             </v>
-      </c>
-      <c r="C32" s="12">
+    <row r="32" spans="2:18" s="33" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B32" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="32">
         <v>5059</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="32">
         <v>4600</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="32">
         <v>4615</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="32">
         <v>5596</v>
       </c>
-      <c r="G32" s="12">
+      <c r="G32" s="32">
         <v>5258</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="32">
         <v>5517</v>
       </c>
-      <c r="I32" s="12">
+      <c r="I32" s="32">
         <v>5517</v>
       </c>
-      <c r="J32" s="12">
+      <c r="J32" s="32">
         <v>5342</v>
       </c>
-      <c r="K32" s="12">
+      <c r="K32" s="32">
         <v>5163</v>
       </c>
-      <c r="L32" s="12">
+      <c r="L32" s="32">
         <v>5882</v>
       </c>
-      <c r="M32" s="12">
+      <c r="M32" s="32">
         <v>5817</v>
       </c>
-      <c r="N32" s="12">
+      <c r="N32" s="32">
         <v>7351</v>
       </c>
-      <c r="O32" s="12">
+      <c r="O32" s="32">
         <v>5946</v>
       </c>
-      <c r="P32" s="12">
+      <c r="P32" s="32">
         <v>6360</v>
       </c>
-      <c r="Q32" s="12">
+      <c r="Q32" s="32">
         <v>6229</v>
       </c>
-      <c r="R32" s="12">
+      <c r="R32" s="32">
         <v>4526</v>
       </c>
     </row>
     <row r="33" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B33" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B26</f>
-        <v xml:space="preserve">  China                     </v>
+      <c r="B33" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="C33" s="15">
         <v>962</v>
@@ -2317,118 +2228,115 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="34" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B27</f>
-        <v xml:space="preserve">Australien und Ozeanien     </v>
-      </c>
-      <c r="C34" s="12">
+    <row r="34" spans="2:18" s="33" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="32">
         <v>396</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="32">
         <v>413</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="32">
         <v>502</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="32">
         <v>608</v>
       </c>
-      <c r="G34" s="12">
+      <c r="G34" s="32">
         <v>562</v>
       </c>
-      <c r="H34" s="12">
+      <c r="H34" s="32">
         <v>547</v>
       </c>
-      <c r="I34" s="12">
+      <c r="I34" s="32">
         <v>535</v>
       </c>
-      <c r="J34" s="12">
+      <c r="J34" s="32">
         <v>500</v>
       </c>
-      <c r="K34" s="12">
+      <c r="K34" s="32">
         <v>554</v>
       </c>
-      <c r="L34" s="12">
+      <c r="L34" s="32">
         <v>572</v>
       </c>
-      <c r="M34" s="12">
+      <c r="M34" s="32">
         <v>531</v>
       </c>
-      <c r="N34" s="12">
+      <c r="N34" s="32">
         <v>593</v>
       </c>
-      <c r="O34" s="12">
+      <c r="O34" s="32">
         <v>566</v>
       </c>
-      <c r="P34" s="12">
+      <c r="P34" s="32">
         <v>524</v>
       </c>
-      <c r="Q34" s="12">
+      <c r="Q34" s="32">
         <v>497</v>
       </c>
-      <c r="R34" s="12">
+      <c r="R34" s="32">
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B35" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B28</f>
-        <v xml:space="preserve">Sonstige Ziele              </v>
-      </c>
-      <c r="C35" s="15">
+    <row r="35" spans="2:18" s="36" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B35" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="35">
         <v>2997</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="35">
         <v>2129</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="35">
         <v>2314</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="35">
         <v>2739</v>
       </c>
-      <c r="G35" s="15">
+      <c r="G35" s="35">
         <v>3003</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H35" s="35">
         <v>2904</v>
       </c>
-      <c r="I35" s="15">
+      <c r="I35" s="35">
         <v>2615</v>
       </c>
-      <c r="J35" s="15">
+      <c r="J35" s="35">
         <v>2812</v>
       </c>
-      <c r="K35" s="15">
+      <c r="K35" s="35">
         <v>1990</v>
       </c>
-      <c r="L35" s="15">
+      <c r="L35" s="35">
         <v>1927</v>
       </c>
-      <c r="M35" s="15">
+      <c r="M35" s="35">
         <v>3002</v>
       </c>
-      <c r="N35" s="15">
+      <c r="N35" s="35">
         <v>29314</v>
       </c>
-      <c r="O35" s="15">
+      <c r="O35" s="35">
         <v>18898</v>
       </c>
-      <c r="P35" s="15">
+      <c r="P35" s="35">
         <v>17345</v>
       </c>
-      <c r="Q35" s="15">
+      <c r="Q35" s="35">
         <v>18248</v>
       </c>
-      <c r="R35" s="15">
+      <c r="R35" s="35">
         <v>14276</v>
       </c>
     </row>
     <row r="36" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B36" s="14" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B29</f>
-        <v xml:space="preserve">  ohne Angabe               </v>
+      <c r="B36" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="C36" s="15">
         <v>0</v>
@@ -2480,9 +2388,8 @@
       </c>
     </row>
     <row r="37" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="str">
-        <f>'[1]2020_1-4-3_Rohdaten'!B30</f>
-        <v xml:space="preserve">Insgesamt                   </v>
+      <c r="B37" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="C37" s="12">
         <v>55376</v>
@@ -2538,7 +2445,7 @@
     </row>
     <row r="39" spans="2:18" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="19" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -2572,7 +2479,7 @@
     </row>
     <row r="41" spans="2:18" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D41" s="23"/>
       <c r="E41" s="21"/>
@@ -2611,5 +2518,6 @@
     <mergeCell ref="C8:R8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 55edec3ef2564767d4e4bd2170def8745e0f43f6 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-4-2.xlsx
+++ b/assets/excel/2021_1-4-2.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D1029D-7521-4FF3-B7FE-BB295010CB0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906E189D-795E-4D74-B35B-0184E5664CAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{5B9D5FF7-0EDA-4F75-B44C-924FC8B4E454}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,9 +28,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
+  </si>
+  <si>
+    <r>
+      <t>Wanderungsherkunft</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="6"/>
+        <rFont val="NDSFrutiger 45 Light"/>
+      </rPr>
+      <t>1)</t>
+    </r>
   </si>
   <si>
     <t>Fortzüge über die Bundesgrenzen aus Niedersachsen</t>
@@ -87,6 +103,9 @@
     <t>17</t>
   </si>
   <si>
+    <t>1) Aufgeführt sind die 20 häufigsten Wanderungsziele im Jahr 2019 als darunter Positionen der in der Zeile Ingesamt augewiesenen Werte "Staatenlos" sowie "ungeklärt und ohne Angabe" werden in Sonstige Ziele geführt.</t>
+  </si>
+  <si>
     <t>Quelle: Wanderungsstatistik</t>
   </si>
   <si>
@@ -97,106 +116,6 @@
   </si>
   <si>
     <t>Tabelle: 1.4.2: Fortzüge über die Bundesgrenzen nach Niedersachsen nach Wanderungsziel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Europa insgesamt            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Albanien                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Bulgarien                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Griechenland              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Italien                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Kosovo                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Moldau, Republik          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Polen                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Rumänien                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Russische Föderation      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Serbien  (ab 2008)        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Spanien                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Türkei                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Ukraine                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EU Staaten                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afrika insgesamt            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amerika insgesamt           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asien insgesamt             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Afghanistan               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Indien                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Irak                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Iran,Islamische Republik  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Kasachstan                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Libanon                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Syrien, Arabische Republik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Australien und Ozeanien     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sonstige Ziele              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insgesamt                   </t>
-  </si>
-  <si>
-    <r>
-      <t>Wanderungsziel</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="6"/>
-        <rFont val="NDSFrutiger 45 Light"/>
-      </rPr>
-      <t>1)</t>
-    </r>
-  </si>
-  <si>
-    <t>1) Aufgeführt sind die 20 häufigsten Wanderungsziele im Jahr 2020 als darunter Positionen der in der Zeile Ingesamt augewiesenen Werte "Staatenlos" sowie "ungeklärt und ohne Angabe" werden in Sonstige Ziele geführt.</t>
   </si>
 </sst>
 </file>
@@ -335,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -415,20 +334,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -444,6 +349,166 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="2020_1-4-3_Download"/>
+      <sheetName val="2020_1-4-3_Rohdaten"/>
+      <sheetName val="2020_1-4-3_CSV_Vorbereitung"/>
+      <sheetName val="2020_1-4-3_CSV_Export"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="B3" t="str">
+            <v xml:space="preserve">Europa insgesamt            </v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v xml:space="preserve">  Bulgarien                 </v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v xml:space="preserve">  Griechenland              </v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v xml:space="preserve">  Italien                   </v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v xml:space="preserve">  Kroatien                  </v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v xml:space="preserve">  Litauen                   </v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v xml:space="preserve">  Moldau, Republik          </v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v xml:space="preserve">  Niederlande               </v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v xml:space="preserve">  Österreich                </v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12" t="str">
+            <v xml:space="preserve">  Polen                     </v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13" t="str">
+            <v xml:space="preserve">  Rumänien                  </v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14" t="str">
+            <v xml:space="preserve">  Schweiz                   </v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15" t="str">
+            <v xml:space="preserve">  Serbien     (ab 2008)</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16" t="str">
+            <v xml:space="preserve">  Spanien                   </v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17" t="str">
+            <v xml:space="preserve">  Türkei                    </v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18" t="str">
+            <v xml:space="preserve">  Ukraine                   </v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19" t="str">
+            <v xml:space="preserve">  Ungarn                    </v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20" t="str">
+            <v xml:space="preserve">  Vereinigtes Königreich, Nordirland</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21" t="str">
+            <v xml:space="preserve"> EU Staaten                 </v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22" t="str">
+            <v xml:space="preserve">Afrika insgesamt            </v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23" t="str">
+            <v xml:space="preserve">Amerika insgesamt           </v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24" t="str">
+            <v xml:space="preserve">  Vereinigte Staaten        </v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v xml:space="preserve">Asien insgesamt             </v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26" t="str">
+            <v xml:space="preserve">  China                     </v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27" t="str">
+            <v xml:space="preserve">Australien und Ozeanien     </v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v xml:space="preserve">Sonstige Ziele              </v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29" t="str">
+            <v xml:space="preserve">  ohne Angabe               </v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="B30" t="str">
+            <v xml:space="preserve">Insgesamt                   </v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -747,7 +812,7 @@
   <dimension ref="B1:R42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +829,7 @@
     <row r="2" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
@@ -780,7 +845,7 @@
     </row>
     <row r="4" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -810,10 +875,10 @@
     </row>
     <row r="6" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
@@ -885,7 +950,7 @@
     <row r="8" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="26"/>
       <c r="C8" s="29" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
@@ -905,60 +970,61 @@
     </row>
     <row r="9" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R9" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
-        <v>24</v>
+      <c r="B10" s="11" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B3</f>
+        <v xml:space="preserve">Europa insgesamt            </v>
       </c>
       <c r="C10" s="12">
         <v>41701</v>
@@ -1010,8 +1076,9 @@
       </c>
     </row>
     <row r="11" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B11" s="14" t="s">
-        <v>25</v>
+      <c r="B11" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B4</f>
+        <v xml:space="preserve">  Bulgarien                 </v>
       </c>
       <c r="C11" s="15">
         <v>396</v>
@@ -1063,8 +1130,9 @@
       </c>
     </row>
     <row r="12" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B12" s="14" t="s">
-        <v>26</v>
+      <c r="B12" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B5</f>
+        <v xml:space="preserve">  Griechenland              </v>
       </c>
       <c r="C12" s="15">
         <v>1008</v>
@@ -1116,8 +1184,9 @@
       </c>
     </row>
     <row r="13" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B13" s="14" t="s">
-        <v>27</v>
+      <c r="B13" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B6</f>
+        <v xml:space="preserve">  Italien                   </v>
       </c>
       <c r="C13" s="15">
         <v>1375</v>
@@ -1169,8 +1238,9 @@
       </c>
     </row>
     <row r="14" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B14" s="14" t="s">
-        <v>28</v>
+      <c r="B14" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B7</f>
+        <v xml:space="preserve">  Kroatien                  </v>
       </c>
       <c r="C14" s="15">
         <v>438</v>
@@ -1222,8 +1292,9 @@
       </c>
     </row>
     <row r="15" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B15" s="14" t="s">
-        <v>29</v>
+      <c r="B15" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B8</f>
+        <v xml:space="preserve">  Litauen                   </v>
       </c>
       <c r="C15" s="15">
         <v>321</v>
@@ -1275,8 +1346,9 @@
       </c>
     </row>
     <row r="16" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B16" s="14" t="s">
-        <v>30</v>
+      <c r="B16" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B9</f>
+        <v xml:space="preserve">  Moldau, Republik          </v>
       </c>
       <c r="C16" s="15">
         <v>34</v>
@@ -1328,8 +1400,9 @@
       </c>
     </row>
     <row r="17" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B17" s="14" t="s">
-        <v>31</v>
+      <c r="B17" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B10</f>
+        <v xml:space="preserve">  Niederlande               </v>
       </c>
       <c r="C17" s="15">
         <v>1191</v>
@@ -1381,8 +1454,9 @@
       </c>
     </row>
     <row r="18" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B18" s="14" t="s">
-        <v>32</v>
+      <c r="B18" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B11</f>
+        <v xml:space="preserve">  Österreich                </v>
       </c>
       <c r="C18" s="15">
         <v>804</v>
@@ -1434,8 +1508,9 @@
       </c>
     </row>
     <row r="19" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B19" s="14" t="s">
-        <v>33</v>
+      <c r="B19" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B12</f>
+        <v xml:space="preserve">  Polen                     </v>
       </c>
       <c r="C19" s="15">
         <v>20880</v>
@@ -1487,8 +1562,9 @@
       </c>
     </row>
     <row r="20" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B20" s="14" t="s">
-        <v>34</v>
+      <c r="B20" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B13</f>
+        <v xml:space="preserve">  Rumänien                  </v>
       </c>
       <c r="C20" s="15">
         <v>584</v>
@@ -1540,8 +1616,9 @@
       </c>
     </row>
     <row r="21" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B21" s="14" t="s">
-        <v>35</v>
+      <c r="B21" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B14</f>
+        <v xml:space="preserve">  Schweiz                   </v>
       </c>
       <c r="C21" s="15">
         <v>771</v>
@@ -1593,17 +1670,18 @@
       </c>
     </row>
     <row r="22" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B22" s="14" t="s">
-        <v>36</v>
+      <c r="B22" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B15</f>
+        <v xml:space="preserve">  Serbien     (ab 2008)</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F22" s="15">
         <v>193</v>
@@ -1646,8 +1724,9 @@
       </c>
     </row>
     <row r="23" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B23" s="14" t="s">
-        <v>37</v>
+      <c r="B23" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B16</f>
+        <v xml:space="preserve">  Spanien                   </v>
       </c>
       <c r="C23" s="15">
         <v>1446</v>
@@ -1698,380 +1777,388 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="24" spans="2:18" s="36" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B24" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="35">
+    <row r="24" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B24" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B17</f>
+        <v xml:space="preserve">  Türkei                    </v>
+      </c>
+      <c r="C24" s="15">
         <v>2012</v>
       </c>
-      <c r="D24" s="35">
+      <c r="D24" s="15">
         <v>2046</v>
       </c>
-      <c r="E24" s="35">
+      <c r="E24" s="15">
         <v>1889</v>
       </c>
-      <c r="F24" s="35">
+      <c r="F24" s="15">
         <v>2159</v>
       </c>
-      <c r="G24" s="35">
+      <c r="G24" s="15">
         <v>2076</v>
       </c>
-      <c r="H24" s="35">
+      <c r="H24" s="15">
         <v>1817</v>
       </c>
-      <c r="I24" s="35">
+      <c r="I24" s="15">
         <v>1727</v>
       </c>
-      <c r="J24" s="35">
+      <c r="J24" s="15">
         <v>1743</v>
       </c>
-      <c r="K24" s="35">
+      <c r="K24" s="15">
         <v>1809</v>
       </c>
-      <c r="L24" s="35">
+      <c r="L24" s="15">
         <v>1821</v>
       </c>
-      <c r="M24" s="35">
+      <c r="M24" s="15">
         <v>1644</v>
       </c>
-      <c r="N24" s="35">
+      <c r="N24" s="15">
         <v>1926</v>
       </c>
-      <c r="O24" s="35">
+      <c r="O24" s="15">
         <v>1636</v>
       </c>
-      <c r="P24" s="35">
+      <c r="P24" s="15">
         <v>1901</v>
       </c>
-      <c r="Q24" s="35">
+      <c r="Q24" s="15">
         <v>1769</v>
       </c>
-      <c r="R24" s="35">
+      <c r="R24" s="15">
         <v>1395</v>
       </c>
     </row>
-    <row r="25" spans="2:18" s="36" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B25" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="35">
+    <row r="25" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B25" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B18</f>
+        <v xml:space="preserve">  Ukraine                   </v>
+      </c>
+      <c r="C25" s="15">
         <v>441</v>
       </c>
-      <c r="D25" s="35">
+      <c r="D25" s="15">
         <v>395</v>
       </c>
-      <c r="E25" s="35">
+      <c r="E25" s="15">
         <v>329</v>
       </c>
-      <c r="F25" s="35">
+      <c r="F25" s="15">
         <v>451</v>
       </c>
-      <c r="G25" s="35">
+      <c r="G25" s="15">
         <v>293</v>
       </c>
-      <c r="H25" s="35">
+      <c r="H25" s="15">
         <v>242</v>
       </c>
-      <c r="I25" s="35">
+      <c r="I25" s="15">
         <v>293</v>
       </c>
-      <c r="J25" s="35">
+      <c r="J25" s="15">
         <v>261</v>
       </c>
-      <c r="K25" s="35">
+      <c r="K25" s="15">
         <v>252</v>
       </c>
-      <c r="L25" s="35">
+      <c r="L25" s="15">
         <v>284</v>
       </c>
-      <c r="M25" s="35">
+      <c r="M25" s="15">
         <v>317</v>
       </c>
-      <c r="N25" s="35">
+      <c r="N25" s="15">
         <v>478</v>
       </c>
-      <c r="O25" s="35">
+      <c r="O25" s="15">
         <v>708</v>
       </c>
-      <c r="P25" s="35">
+      <c r="P25" s="15">
         <v>683</v>
       </c>
-      <c r="Q25" s="35">
+      <c r="Q25" s="15">
         <v>1070</v>
       </c>
-      <c r="R25" s="35">
+      <c r="R25" s="15">
         <v>752</v>
       </c>
     </row>
-    <row r="26" spans="2:18" s="36" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B26" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="35">
+    <row r="26" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B26" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B19</f>
+        <v xml:space="preserve">  Ungarn                    </v>
+      </c>
+      <c r="C26" s="15">
         <v>1435</v>
       </c>
-      <c r="D26" s="35">
+      <c r="D26" s="15">
         <v>1719</v>
       </c>
-      <c r="E26" s="35">
+      <c r="E26" s="15">
         <v>2058</v>
       </c>
-      <c r="F26" s="35">
+      <c r="F26" s="15">
         <v>2415</v>
       </c>
-      <c r="G26" s="35">
+      <c r="G26" s="15">
         <v>2632</v>
       </c>
-      <c r="H26" s="35">
+      <c r="H26" s="15">
         <v>2054</v>
       </c>
-      <c r="I26" s="35">
+      <c r="I26" s="15">
         <v>2534</v>
       </c>
-      <c r="J26" s="35">
+      <c r="J26" s="15">
         <v>2651</v>
       </c>
-      <c r="K26" s="35">
+      <c r="K26" s="15">
         <v>3419</v>
       </c>
-      <c r="L26" s="35">
+      <c r="L26" s="15">
         <v>3489</v>
       </c>
-      <c r="M26" s="35">
+      <c r="M26" s="15">
         <v>2997</v>
       </c>
-      <c r="N26" s="35">
+      <c r="N26" s="15">
         <v>3035</v>
       </c>
-      <c r="O26" s="35">
+      <c r="O26" s="15">
         <v>2765</v>
       </c>
-      <c r="P26" s="35">
+      <c r="P26" s="15">
         <v>2578</v>
       </c>
-      <c r="Q26" s="35">
+      <c r="Q26" s="15">
         <v>2332</v>
       </c>
-      <c r="R26" s="35">
+      <c r="R26" s="15">
         <v>2020</v>
       </c>
     </row>
-    <row r="27" spans="2:18" s="36" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B27" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="35">
+    <row r="27" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B27" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B20</f>
+        <v xml:space="preserve">  Vereinigtes Königreich, Nordirland</v>
+      </c>
+      <c r="C27" s="15">
         <v>1329</v>
       </c>
-      <c r="D27" s="35">
+      <c r="D27" s="15">
         <v>1428</v>
       </c>
-      <c r="E27" s="35">
+      <c r="E27" s="15">
         <v>1242</v>
       </c>
-      <c r="F27" s="35">
+      <c r="F27" s="15">
         <v>1434</v>
       </c>
-      <c r="G27" s="35">
+      <c r="G27" s="15">
         <v>1435</v>
       </c>
-      <c r="H27" s="35">
+      <c r="H27" s="15">
         <v>1176</v>
       </c>
-      <c r="I27" s="35">
+      <c r="I27" s="15">
         <v>1276</v>
       </c>
-      <c r="J27" s="35">
+      <c r="J27" s="15">
         <v>1177</v>
       </c>
-      <c r="K27" s="35">
+      <c r="K27" s="15">
         <v>1227</v>
       </c>
-      <c r="L27" s="35">
+      <c r="L27" s="15">
         <v>1531</v>
       </c>
-      <c r="M27" s="35">
+      <c r="M27" s="15">
         <v>1497</v>
       </c>
-      <c r="N27" s="35">
+      <c r="N27" s="15">
         <v>1339</v>
       </c>
-      <c r="O27" s="35">
+      <c r="O27" s="15">
         <v>1090</v>
       </c>
-      <c r="P27" s="35">
+      <c r="P27" s="15">
         <v>1193</v>
       </c>
-      <c r="Q27" s="35">
+      <c r="Q27" s="15">
         <v>1200</v>
       </c>
-      <c r="R27" s="35">
+      <c r="R27" s="15">
         <v>887</v>
       </c>
     </row>
-    <row r="28" spans="2:18" s="33" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="32">
+    <row r="28" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B21</f>
+        <v xml:space="preserve"> EU Staaten                 </v>
+      </c>
+      <c r="C28" s="12">
         <v>35054</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="12">
         <v>37538</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="12">
         <v>40122</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="12">
         <v>44373</v>
       </c>
-      <c r="G28" s="32">
+      <c r="G28" s="12">
         <v>44947</v>
       </c>
-      <c r="H28" s="32">
+      <c r="H28" s="12">
         <v>41807</v>
       </c>
-      <c r="I28" s="32">
+      <c r="I28" s="12">
         <v>47208</v>
       </c>
-      <c r="J28" s="32">
+      <c r="J28" s="12">
         <v>50761</v>
       </c>
-      <c r="K28" s="32">
+      <c r="K28" s="12">
         <v>55590</v>
       </c>
-      <c r="L28" s="32">
+      <c r="L28" s="12">
         <v>61810</v>
       </c>
-      <c r="M28" s="32">
+      <c r="M28" s="12">
         <v>58568</v>
       </c>
-      <c r="N28" s="32">
+      <c r="N28" s="12">
         <v>68721</v>
       </c>
-      <c r="O28" s="32">
+      <c r="O28" s="12">
         <v>62569</v>
       </c>
-      <c r="P28" s="32">
+      <c r="P28" s="12">
         <v>69033</v>
       </c>
-      <c r="Q28" s="32">
+      <c r="Q28" s="12">
         <v>71647</v>
       </c>
-      <c r="R28" s="32">
+      <c r="R28" s="12">
         <v>55071</v>
       </c>
     </row>
-    <row r="29" spans="2:18" s="33" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="32">
+    <row r="29" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B22</f>
+        <v xml:space="preserve">Afrika insgesamt            </v>
+      </c>
+      <c r="C29" s="12">
         <v>1545</v>
       </c>
-      <c r="D29" s="32">
+      <c r="D29" s="12">
         <v>1512</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="12">
         <v>1367</v>
       </c>
-      <c r="F29" s="32">
+      <c r="F29" s="12">
         <v>1598</v>
       </c>
-      <c r="G29" s="32">
+      <c r="G29" s="12">
         <v>1348</v>
       </c>
-      <c r="H29" s="32">
+      <c r="H29" s="12">
         <v>1208</v>
       </c>
-      <c r="I29" s="32">
+      <c r="I29" s="12">
         <v>1259</v>
       </c>
-      <c r="J29" s="32">
+      <c r="J29" s="12">
         <v>1257</v>
       </c>
-      <c r="K29" s="32">
+      <c r="K29" s="12">
         <v>1355</v>
       </c>
-      <c r="L29" s="32">
+      <c r="L29" s="12">
         <v>2023</v>
       </c>
-      <c r="M29" s="32">
+      <c r="M29" s="12">
         <v>2438</v>
       </c>
-      <c r="N29" s="32">
+      <c r="N29" s="12">
         <v>6689</v>
       </c>
-      <c r="O29" s="32">
+      <c r="O29" s="12">
         <v>4200</v>
       </c>
-      <c r="P29" s="32">
+      <c r="P29" s="12">
         <v>2701</v>
       </c>
-      <c r="Q29" s="32">
+      <c r="Q29" s="12">
         <v>2560</v>
       </c>
-      <c r="R29" s="32">
+      <c r="R29" s="12">
         <v>2013</v>
       </c>
     </row>
-    <row r="30" spans="2:18" s="33" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B30" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="32">
+    <row r="30" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B23</f>
+        <v xml:space="preserve">Amerika insgesamt           </v>
+      </c>
+      <c r="C30" s="12">
         <v>3678</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D30" s="12">
         <v>3627</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="12">
         <v>4031</v>
       </c>
-      <c r="F30" s="32">
+      <c r="F30" s="12">
         <v>5228</v>
       </c>
-      <c r="G30" s="32">
+      <c r="G30" s="12">
         <v>4375</v>
       </c>
-      <c r="H30" s="32">
+      <c r="H30" s="12">
         <v>4047</v>
       </c>
-      <c r="I30" s="32">
+      <c r="I30" s="12">
         <v>4034</v>
       </c>
-      <c r="J30" s="32">
+      <c r="J30" s="12">
         <v>3832</v>
       </c>
-      <c r="K30" s="32">
+      <c r="K30" s="12">
         <v>3847</v>
       </c>
-      <c r="L30" s="32">
+      <c r="L30" s="12">
         <v>4067</v>
       </c>
-      <c r="M30" s="32">
+      <c r="M30" s="12">
         <v>3859</v>
       </c>
-      <c r="N30" s="32">
+      <c r="N30" s="12">
         <v>4286</v>
       </c>
-      <c r="O30" s="32">
+      <c r="O30" s="12">
         <v>3611</v>
       </c>
-      <c r="P30" s="32">
+      <c r="P30" s="12">
         <v>3577</v>
       </c>
-      <c r="Q30" s="32">
+      <c r="Q30" s="12">
         <v>3820</v>
       </c>
-      <c r="R30" s="32">
+      <c r="R30" s="12">
         <v>2624</v>
       </c>
     </row>
     <row r="31" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B31" s="14" t="s">
-        <v>45</v>
+      <c r="B31" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B24</f>
+        <v xml:space="preserve">  Vereinigte Staaten        </v>
       </c>
       <c r="C31" s="15">
         <v>1677</v>
@@ -2122,62 +2209,64 @@
         <v>958</v>
       </c>
     </row>
-    <row r="32" spans="2:18" s="33" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B32" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="32">
+    <row r="32" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B25</f>
+        <v xml:space="preserve">Asien insgesamt             </v>
+      </c>
+      <c r="C32" s="12">
         <v>5059</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D32" s="12">
         <v>4600</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="12">
         <v>4615</v>
       </c>
-      <c r="F32" s="32">
+      <c r="F32" s="12">
         <v>5596</v>
       </c>
-      <c r="G32" s="32">
+      <c r="G32" s="12">
         <v>5258</v>
       </c>
-      <c r="H32" s="32">
+      <c r="H32" s="12">
         <v>5517</v>
       </c>
-      <c r="I32" s="32">
+      <c r="I32" s="12">
         <v>5517</v>
       </c>
-      <c r="J32" s="32">
+      <c r="J32" s="12">
         <v>5342</v>
       </c>
-      <c r="K32" s="32">
+      <c r="K32" s="12">
         <v>5163</v>
       </c>
-      <c r="L32" s="32">
+      <c r="L32" s="12">
         <v>5882</v>
       </c>
-      <c r="M32" s="32">
+      <c r="M32" s="12">
         <v>5817</v>
       </c>
-      <c r="N32" s="32">
+      <c r="N32" s="12">
         <v>7351</v>
       </c>
-      <c r="O32" s="32">
+      <c r="O32" s="12">
         <v>5946</v>
       </c>
-      <c r="P32" s="32">
+      <c r="P32" s="12">
         <v>6360</v>
       </c>
-      <c r="Q32" s="32">
+      <c r="Q32" s="12">
         <v>6229</v>
       </c>
-      <c r="R32" s="32">
+      <c r="R32" s="12">
         <v>4526</v>
       </c>
     </row>
     <row r="33" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B33" s="14" t="s">
-        <v>47</v>
+      <c r="B33" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B26</f>
+        <v xml:space="preserve">  China                     </v>
       </c>
       <c r="C33" s="15">
         <v>962</v>
@@ -2228,115 +2317,118 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="34" spans="2:18" s="33" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B34" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="32">
+    <row r="34" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B27</f>
+        <v xml:space="preserve">Australien und Ozeanien     </v>
+      </c>
+      <c r="C34" s="12">
         <v>396</v>
       </c>
-      <c r="D34" s="32">
+      <c r="D34" s="12">
         <v>413</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="12">
         <v>502</v>
       </c>
-      <c r="F34" s="32">
+      <c r="F34" s="12">
         <v>608</v>
       </c>
-      <c r="G34" s="32">
+      <c r="G34" s="12">
         <v>562</v>
       </c>
-      <c r="H34" s="32">
+      <c r="H34" s="12">
         <v>547</v>
       </c>
-      <c r="I34" s="32">
+      <c r="I34" s="12">
         <v>535</v>
       </c>
-      <c r="J34" s="32">
+      <c r="J34" s="12">
         <v>500</v>
       </c>
-      <c r="K34" s="32">
+      <c r="K34" s="12">
         <v>554</v>
       </c>
-      <c r="L34" s="32">
+      <c r="L34" s="12">
         <v>572</v>
       </c>
-      <c r="M34" s="32">
+      <c r="M34" s="12">
         <v>531</v>
       </c>
-      <c r="N34" s="32">
+      <c r="N34" s="12">
         <v>593</v>
       </c>
-      <c r="O34" s="32">
+      <c r="O34" s="12">
         <v>566</v>
       </c>
-      <c r="P34" s="32">
+      <c r="P34" s="12">
         <v>524</v>
       </c>
-      <c r="Q34" s="32">
+      <c r="Q34" s="12">
         <v>497</v>
       </c>
-      <c r="R34" s="32">
+      <c r="R34" s="12">
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="2:18" s="36" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B35" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="35">
+    <row r="35" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+      <c r="B35" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B28</f>
+        <v xml:space="preserve">Sonstige Ziele              </v>
+      </c>
+      <c r="C35" s="15">
         <v>2997</v>
       </c>
-      <c r="D35" s="35">
+      <c r="D35" s="15">
         <v>2129</v>
       </c>
-      <c r="E35" s="35">
+      <c r="E35" s="15">
         <v>2314</v>
       </c>
-      <c r="F35" s="35">
+      <c r="F35" s="15">
         <v>2739</v>
       </c>
-      <c r="G35" s="35">
+      <c r="G35" s="15">
         <v>3003</v>
       </c>
-      <c r="H35" s="35">
+      <c r="H35" s="15">
         <v>2904</v>
       </c>
-      <c r="I35" s="35">
+      <c r="I35" s="15">
         <v>2615</v>
       </c>
-      <c r="J35" s="35">
+      <c r="J35" s="15">
         <v>2812</v>
       </c>
-      <c r="K35" s="35">
+      <c r="K35" s="15">
         <v>1990</v>
       </c>
-      <c r="L35" s="35">
+      <c r="L35" s="15">
         <v>1927</v>
       </c>
-      <c r="M35" s="35">
+      <c r="M35" s="15">
         <v>3002</v>
       </c>
-      <c r="N35" s="35">
+      <c r="N35" s="15">
         <v>29314</v>
       </c>
-      <c r="O35" s="35">
+      <c r="O35" s="15">
         <v>18898</v>
       </c>
-      <c r="P35" s="35">
+      <c r="P35" s="15">
         <v>17345</v>
       </c>
-      <c r="Q35" s="35">
+      <c r="Q35" s="15">
         <v>18248</v>
       </c>
-      <c r="R35" s="35">
+      <c r="R35" s="15">
         <v>14276</v>
       </c>
     </row>
     <row r="36" spans="2:18" s="16" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
-      <c r="B36" s="14" t="s">
-        <v>50</v>
+      <c r="B36" s="14" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B29</f>
+        <v xml:space="preserve">  ohne Angabe               </v>
       </c>
       <c r="C36" s="15">
         <v>0</v>
@@ -2388,8 +2480,9 @@
       </c>
     </row>
     <row r="37" spans="2:18" s="13" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="s">
-        <v>51</v>
+      <c r="B37" s="11" t="str">
+        <f>'[1]2020_1-4-3_Rohdaten'!B30</f>
+        <v xml:space="preserve">Insgesamt                   </v>
       </c>
       <c r="C37" s="12">
         <v>55376</v>
@@ -2445,7 +2538,7 @@
     </row>
     <row r="39" spans="2:18" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="19" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -2479,7 +2572,7 @@
     </row>
     <row r="41" spans="2:18" s="18" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="22" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D41" s="23"/>
       <c r="E41" s="21"/>
@@ -2518,6 +2611,5 @@
     <mergeCell ref="C8:R8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>